<commit_message>
Rédaction de la première partie du TP !!
Une super ptite soirée de 8h !!
En tout cas je suis prêt à passer à la suite, ma VM est prête avec vagrant & PuPHP :)
ya plus qu'à attaquer la partie 2 !!
</commit_message>
<xml_diff>
--- a/Documentation/Classeur.xlsx
+++ b/Documentation/Classeur.xlsx
@@ -3,21 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\School\PolyMtl\Java\TP1_INF4410_1761581\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162912"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>10ei</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>local</t>
   </si>
@@ -27,12 +29,31 @@
   <si>
     <t>distant RMI</t>
   </si>
+  <si>
+    <t>local (µs)</t>
+  </si>
+  <si>
+    <t>local RMI (µs)</t>
+  </si>
+  <si>
+    <t>distant RMI (µs)</t>
+  </si>
+  <si>
+    <t>nb octets</t>
+  </si>
+  <si>
+    <t>moyenne</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0E+00"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,16 +61,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -57,17 +106,243 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="169" formatCode="0E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0E+00"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -94,15 +369,104 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>temps moyen réponse (µs) = f(taille argument en octets)</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR" sz="800">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14758791903148857"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14208612812287352"/>
+          <c:y val="9.5937278226487788E-2"/>
+          <c:w val="0.77328906536255615"/>
+          <c:h val="0.72052403320829528"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>local</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -131,31 +495,31 @@
             <c:numRef>
               <c:f>Feuil1!$A$2:$A$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0E+00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>10000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>100000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>1000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -167,42 +531,48 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>170</c:v>
+                  <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>138</c:v>
+                  <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>138</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>189917</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>111</c:v>
+                  <c:v>406</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>251</c:v>
+                  <c:v>485</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>137</c:v>
+                  <c:v>442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3D23-41F2-8B4D-16ACD1A620A9}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>local RMI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -231,31 +601,31 @@
             <c:numRef>
               <c:f>Feuil1!$A$2:$A$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0E+00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>10000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>100000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>1000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -294,15 +664,21 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3D23-41F2-8B4D-16ACD1A620A9}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>distant RMI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -331,31 +707,31 @@
             <c:numRef>
               <c:f>Feuil1!$A$2:$A$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0E+00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>10000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>100000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>1000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -394,11 +770,6 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3D23-41F2-8B4D-16ACD1A620A9}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -408,13 +779,16 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1284992072"/>
-        <c:axId val="1284990280"/>
+        <c:axId val="350676648"/>
+        <c:axId val="350676256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1284992072"/>
+        <c:axId val="350676648"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:max val="1000000000"/>
+          <c:min val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -432,7 +806,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -466,15 +840,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1284990280"/>
+        <c:crossAx val="350676256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1284990280"/>
+        <c:axId val="350676256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,12 +902,13 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1284992072"/>
+        <c:crossAx val="350676648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1000000000"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -545,6 +920,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12362249590596047"/>
+          <c:y val="0.90343280051366959"/>
+          <c:w val="0.75275500818807906"/>
+          <c:h val="9.6567199486330302E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -570,7 +955,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -600,7 +985,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -625,15 +1010,123 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1100"/>
+              <a:t>temps moyen</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+              <a:t> réponse (</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>µs</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+              <a:t>) = f(taille argument en octets)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="900" i="1" baseline="0"/>
+              <a:t>échelles logarithmiques</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR" sz="900" i="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21295541783996813"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22018924139237919"/>
+          <c:y val="0.10532051282051282"/>
+          <c:w val="0.54641304133994595"/>
+          <c:h val="0.81068897637795279"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>local (µs)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -658,64 +1151,169 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$A$2:$A$6</c:f>
+              <c:f>Feuil1!$A$14:$A$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:formatCode>0E+00</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$B$2:$B$6</c:f>
+              <c:f>Feuil1!$B$14:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>170</c:v>
+                  <c:v>0.28799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>138</c:v>
+                  <c:v>0.254</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>138</c:v>
+                  <c:v>0.23100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>189917</c:v>
+                  <c:v>0.23100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
+                  <c:v>0.255</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.40600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.48499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BD98-434A-9BD3-3F682E95286B}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$C$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>local RMI (µs)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -740,64 +1338,180 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.3507325192429E-3"/>
+                  <c:y val="1.9230769230769232E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$A$2:$A$6</c:f>
+              <c:f>Feuil1!$A$14:$A$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:formatCode>0E+00</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$C$2:$C$6</c:f>
+              <c:f>Feuil1!$C$14:$C$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>188046</c:v>
+                  <c:v>188.04599999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>160134</c:v>
+                  <c:v>160.13399999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>129725</c:v>
+                  <c:v>129.72499999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>133437</c:v>
+                  <c:v>133.43700000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>248945</c:v>
+                  <c:v>248.94499999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1130.432</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7049.5990000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>74887.243000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BD98-434A-9BD3-3F682E95286B}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$D$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>distant RMI (µs)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -822,60 +1536,226 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.8455127634699948E-2"/>
+                  <c:y val="-2.2435897435897436E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout/>
+              <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$A$2:$A$6</c:f>
+              <c:f>Feuil1!$A$14:$A$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:formatCode>0E+00</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$D$2:$D$6</c:f>
+              <c:f>Feuil1!$D$14:$D$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>820914</c:v>
+                  <c:v>820.91399999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>780697</c:v>
+                  <c:v>780.697</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1060525</c:v>
+                  <c:v>1060.5250000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1725952</c:v>
+                  <c:v>1725.952</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9515734</c:v>
+                  <c:v>9515.7340000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>86208.52</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>853101.245</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8542826.2819999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-BD98-434A-9BD3-3F682E95286B}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -885,13 +1765,16 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1408050056"/>
-        <c:axId val="1339817032"/>
+        <c:axId val="350675080"/>
+        <c:axId val="350672336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1408050056"/>
+        <c:axId val="350675080"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:max val="1000000000"/>
+          <c:min val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -909,8 +1792,229 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" b="0" i="1"/>
+                  <a:t>nb</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" b="0" i="1" baseline="0"/>
+                  <a:t> octets passés en paramêtre - échelle logarithmique</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR" b="0" i="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="350672336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="350672336"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Temps moyen pour 20 itérations (µs)</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="800" i="1"/>
+                  <a:t>échelle logarithmique</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -943,72 +2047,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1339817032"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1339817032"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1408050056"/>
+        <c:crossAx val="350675080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1021,7 +2063,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1047,7 +2090,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1077,7 +2120,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2204,26 +3247,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2008355-515E-4B0F-9C22-A8DF21948C70}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="Graphique 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2240,27 +3277,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B11D5F78-8C2E-44B0-8746-2E504B24A72F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="5" name="Graphique 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2277,15 +3310,52 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D9" totalsRowShown="0">
+  <autoFilter ref="A1:D9"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="nb octets" dataDxfId="11"/>
+    <tableColumn id="2" name="local"/>
+    <tableColumn id="3" name="local RMI"/>
+    <tableColumn id="4" name="distant RMI"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A13:D22" totalsRowCount="1" headerRowDxfId="0" dataDxfId="5" totalsRowDxfId="6" headerRowBorderDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A13:D22"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="nb octets" totalsRowLabel="moyenne" dataDxfId="10" totalsRowDxfId="4">
+      <calculatedColumnFormula>A2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="local (µs)" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="3" dataCellStyle="Milliers">
+      <calculatedColumnFormula>B2/1000</calculatedColumnFormula>
+      <totalsRowFormula>AVERAGE(Tableau2[local (µs)])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" name="local RMI (µs)" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="2" dataCellStyle="Milliers">
+      <calculatedColumnFormula>C2/1000</calculatedColumnFormula>
+      <totalsRowFormula>AVERAGE(Tableau2[local RMI (µs)])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" name="distant RMI (µs)" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="1" dataCellStyle="Milliers">
+      <calculatedColumnFormula>D2/1000</calculatedColumnFormula>
+      <totalsRowFormula>AVERAGE(Tableau2[distant RMI (µs)])</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2540,32 +3610,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>100</v>
       </c>
       <c r="B2">
-        <v>170</v>
+        <v>288</v>
       </c>
       <c r="C2">
         <v>188046</v>
@@ -2574,12 +3652,12 @@
         <v>820914</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>2</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1000</v>
       </c>
       <c r="B3">
-        <v>138</v>
+        <v>254</v>
       </c>
       <c r="C3">
         <v>160134</v>
@@ -2588,12 +3666,12 @@
         <v>780697</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>3</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>10000</v>
       </c>
       <c r="B4">
-        <v>138</v>
+        <v>231</v>
       </c>
       <c r="C4">
         <v>129725</v>
@@ -2602,12 +3680,12 @@
         <v>1060525</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>4</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>100000</v>
       </c>
       <c r="B5">
-        <v>189917</v>
+        <v>231</v>
       </c>
       <c r="C5">
         <v>133437</v>
@@ -2616,12 +3694,12 @@
         <v>1725952</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>5</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1000000</v>
       </c>
       <c r="B6">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="C6">
         <v>248945</v>
@@ -2630,12 +3708,12 @@
         <v>9515734</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>6</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>10000000</v>
       </c>
       <c r="B7">
-        <v>111</v>
+        <v>406</v>
       </c>
       <c r="C7">
         <v>1130432</v>
@@ -2644,12 +3722,12 @@
         <v>86208520</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>7</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>100000000</v>
       </c>
       <c r="B8">
-        <v>251</v>
+        <v>485</v>
       </c>
       <c r="C8">
         <v>7049599</v>
@@ -2658,22 +3736,216 @@
         <v>853101245</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>8</v>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1000000000</v>
       </c>
       <c r="B9">
-        <v>137</v>
+        <v>442</v>
       </c>
       <c r="C9">
         <v>74887243</v>
       </c>
       <c r="D9">
         <v>8542826282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <f>A2</f>
+        <v>100</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" ref="B14:D21" si="0">B2/1000</f>
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="0"/>
+        <v>188.04599999999999</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
+        <v>820.91399999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <f t="shared" ref="A15:A20" si="1">A3</f>
+        <v>1000</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" si="0"/>
+        <v>0.254</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" si="0"/>
+        <v>160.13399999999999</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>780.697</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" si="0"/>
+        <v>129.72499999999999</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
+        <v>1060.5250000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="B17" s="4">
+        <f t="shared" si="0"/>
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" si="0"/>
+        <v>133.43700000000001</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
+        <v>1725.952</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" si="0"/>
+        <v>0.255</v>
+      </c>
+      <c r="C18" s="5">
+        <f t="shared" si="0"/>
+        <v>248.94499999999999</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="0"/>
+        <v>9515.7340000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <f t="shared" si="1"/>
+        <v>10000000</v>
+      </c>
+      <c r="B19" s="4">
+        <f t="shared" si="0"/>
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" si="0"/>
+        <v>1130.432</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
+        <v>86208.52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <f t="shared" si="1"/>
+        <v>100000000</v>
+      </c>
+      <c r="B20" s="4">
+        <f t="shared" si="0"/>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" si="0"/>
+        <v>7049.5990000000002</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" si="0"/>
+        <v>853101.245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <f>A9</f>
+        <v>1000000000</v>
+      </c>
+      <c r="B21" s="4">
+        <f t="shared" si="0"/>
+        <v>0.442</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" si="0"/>
+        <v>74887.243000000002</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="0"/>
+        <v>8542826.2819999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="4">
+        <f>AVERAGE(Tableau2[local (µs)])</f>
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="C22" s="5">
+        <f>AVERAGE(Tableau2[local RMI (µs)])</f>
+        <v>10490.945125</v>
+      </c>
+      <c r="D22" s="5">
+        <f>AVERAGE(Tableau2[distant RMI (µs)])</f>
+        <v>1187004.9836249999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <f>CORREL(C18:C21,A18:A21)</f>
+        <v>0.99995439508513673</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f>CORREL(D17:D21,A17:A21)</f>
+        <v>0.99999997260029394</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>